<commit_message>
#### Upload Data Part working with lots of constraints
</commit_message>
<xml_diff>
--- a/Timetable Uploadable Format.xlsx
+++ b/Timetable Uploadable Format.xlsx
@@ -12,14 +12,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7005"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TT" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171026"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="55">
   <si>
     <t>Time</t>
   </si>
@@ -61,6 +61,129 @@
   </si>
   <si>
     <t>ShortForm</t>
+  </si>
+  <si>
+    <t>Break</t>
+  </si>
+  <si>
+    <t>MCAN</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>DSIP</t>
+  </si>
+  <si>
+    <t>SPCC</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>Open Source</t>
+  </si>
+  <si>
+    <t>Digital Signal and Image Processing</t>
+  </si>
+  <si>
+    <t>System Programming and Compiler Construction</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Audit Course</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>B205</t>
+  </si>
+  <si>
+    <t>B109</t>
+  </si>
+  <si>
+    <t>PCT</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>B115</t>
+  </si>
+  <si>
+    <t>B210A</t>
+  </si>
+  <si>
+    <t>B216</t>
+  </si>
+  <si>
+    <t>Mobile Communication and Ad-Hoc Network</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>PSP</t>
+  </si>
+  <si>
+    <t>PSG</t>
+  </si>
+  <si>
+    <t>K_D</t>
+  </si>
+  <si>
+    <t>SNM</t>
+  </si>
+  <si>
+    <t>KLT</t>
+  </si>
+  <si>
+    <t>GJS</t>
+  </si>
+  <si>
+    <t>V_C</t>
+  </si>
+  <si>
+    <t>PJS</t>
+  </si>
+  <si>
+    <t>Professional Communication Technique</t>
+  </si>
+  <si>
+    <t>09:30:00 AM</t>
+  </si>
+  <si>
+    <t>10:30:00 AM</t>
+  </si>
+  <si>
+    <t>11:30:00 AM</t>
+  </si>
+  <si>
+    <t>12:30:00 PM</t>
+  </si>
+  <si>
+    <t>01:15:00 PM</t>
+  </si>
+  <si>
+    <t>02:15:00 PM</t>
+  </si>
+  <si>
+    <t>03:15:00 PM</t>
+  </si>
+  <si>
+    <t>04:15:00 PM</t>
+  </si>
+  <si>
+    <t>05:15:00 PM</t>
   </si>
 </sst>
 </file>
@@ -96,12 +219,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,173 +550,647 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:U8"/>
+  <dimension ref="A2:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="9" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P3" t="s">
+      <c r="S3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="R3" t="s">
+      <c r="U3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S3" t="s">
+      <c r="W3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="T3" t="s">
+      <c r="X3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="U3" t="s">
+      <c r="Y3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="E4" s="2">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="E5" s="2">
-        <v>0.4375</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.47916666666666669</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="E6" s="2">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.52083333333333337</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="E7" s="2">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.55208333333333337</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H23" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="G2:I2"/>
+  <mergeCells count="34">
+    <mergeCell ref="Y5:Y6"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="U10:U11"/>
+    <mergeCell ref="T10:T11"/>
+    <mergeCell ref="V10:V11"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="X5:X6"/>
+    <mergeCell ref="Z5:Z6"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="Q10:Q11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="P10:P11"/>
+    <mergeCell ref="R10:R11"/>
+    <mergeCell ref="S10:S11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="G2:J2"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:V2"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>